<commit_message>
fixed minimal xlsx by removing header
</commit_message>
<xml_diff>
--- a/g2p/tests/public/mappings/minimal.xlsx
+++ b/g2p/tests/public/mappings/minimal.xlsx
@@ -12,10 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>a</t>
   </si>
@@ -77,12 +74,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -94,28 +91,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -129,7 +104,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -138,7 +113,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -147,43 +122,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -193,32 +153,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -238,12 +189,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1308,7 +1258,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1322,42 +1272,31 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>1</v>
+      <c r="A2" t="s" s="3">
+        <v>2</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s" s="8">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
fix: loading xlsx workbooks should not fail on empty cells
</commit_message>
<xml_diff>
--- a/g2p/tests/public/mappings/minimal.xlsx
+++ b/g2p/tests/public/mappings/minimal.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joanise\sandboxes\g2p\g2p\tests\public\mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79DB959-C4D1-4AF4-BF7C-2A0D5DEC8195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>a</t>
   </si>
@@ -26,28 +34,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -149,27 +144,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -180,27 +175,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -402,7 +455,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -421,7 +474,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -451,7 +504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -477,7 +530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -503,7 +556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +582,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -555,7 +608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -581,7 +634,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -607,7 +660,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -633,7 +686,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -659,7 +712,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -672,9 +725,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -691,7 +750,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -710,7 +769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -736,7 +795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -762,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -788,7 +847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -814,7 +873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -840,7 +899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -866,7 +925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -892,7 +951,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -918,7 +977,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -944,7 +1003,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -957,9 +1016,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -973,7 +1038,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -992,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1022,7 +1087,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1048,7 +1113,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1074,7 +1139,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1126,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1217,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1178,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1243,62 +1308,70 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:IV2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="27.6" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>